<commit_message>
cambiado arbol de directorios. Ya funcando todo el parseo de un pedido normal faltan los combos y las escrituras al consolidado
</commit_message>
<xml_diff>
--- a/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
+++ b/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
@@ -140,17 +140,16 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM"/>
-    <numFmt numFmtId="166" formatCode="D/M/YYYY"/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * \-??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="167" formatCode="\ * #,##0.00\ ;\ * \-#,##0.00\ ;\ * \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -171,15 +170,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -187,7 +196,6 @@
       <color rgb="FF000000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -195,17 +203,15 @@
       <color rgb="FF000000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +226,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFC5C3C3"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
@@ -233,13 +245,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFC5C3C3"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
@@ -345,7 +357,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,183 +371,183 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -558,11 +570,11 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFF2CC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDAE3F3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDAE3F3"/>
+      <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -602,269 +614,25 @@
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Resumen de pedidos"/>
-      <sheetName val="Base de pedidos"/>
-      <sheetName val="Pedido Pency"/>
-      <sheetName val="Productos"/>
-      <sheetName val="Precios y Menú"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="3">
-          <cell r="I3" t="str">
-            <v>BBQ Ribs</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="I4" t="str">
-            <v>Bife de Chorizo al Marsala</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="I5" t="str">
-            <v>Bondiola teriyaki</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6" t="str">
-            <v>
-Matambre a la pizza</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="I7" t="str">
-            <v>Matambrito de cerdo al verdeo</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="I8" t="str">
-            <v>
-Roast beef a la cerveza negra</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="I9" t="str">
-            <v>Solomillo de cerdo laqueado</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="I10" t="str">
-            <v>Premium 8</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="I11" t="str">
-            <v>Premium 9</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="I12" t="str">
-            <v>Premium 10</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="I13" t="str">
-            <v>Gnocchis de papa con goulash</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="I14" t="str">
-            <v>Milanesitas de cerdo a la napolitana</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="I15" t="str">
-            <v>Pata muslo al verdeo</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="I16" t="str">
-            <v>Pollo al ajillo</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="I17" t="str">
-            <v>Spaghetti con puttanesca</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="I18" t="str">
-            <v>Strogonoff de ternera</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="I19" t="str">
-            <v>Suprema con mostaza y miel</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="I20" t="str">
-            <v>Daily 18</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="I21" t="str">
-            <v>Daily 19</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="I22" t="str">
-            <v>Daily 20</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="I23" t="str">
-            <v>Puré de papas</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="I24" t="str">
-            <v>Puré de batatas</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="I25" t="str">
-            <v>Arroz salteado con huevo, sésamo y cebollita de verdeo</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="I26" t="str">
-            <v>Milhojas de papa</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="I27" t="str">
-            <v>Batatas cuña</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="I28" t="str">
-            <v>Cebollas Caramelizadas</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="I29" t="str">
-            <v>Focaccia al romero</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="I30" t="str">
-            <v>Kabutea con puerros</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="I31" t="str">
-            <v>Guarnición 29</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="I32" t="str">
-            <v>Guarnición 30</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="I33" t="str">
-            <v>Guarnición 31</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="I34" t="str">
-            <v>Guarnición 32</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="I35" t="str">
-            <v>Guarnición 33</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="I36" t="str">
-            <v>Guarnición 34</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="I37" t="str">
-            <v>Guarnición 35</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="I38" t="str">
-            <v>Promo 1 Entrada</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="I39" t="str">
-            <v>Promo 1 Principal</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="I40" t="str">
-            <v>Promo 1 Guarnición</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="I41" t="str">
-            <v>Promo 1 Salsas</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="I42" t="str">
-            <v>Promo 1 Bebidas</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="I43" t="str">
-            <v>Promo 2 Entrada</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="I44" t="str">
-            <v>Promo 2 Principal</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="I45" t="str">
-            <v>Promo 2 Guarnición</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="I46" t="str">
-            <v>Promo 2 Salsas</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="I47" t="str">
-            <v>Promo 2 Bebidas</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,7 +657,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -901,31 +669,31 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
@@ -968,7 +736,7 @@
         <f aca="false">+'[1]Precios y Menú'!I3</f>
         <v>BBQ Ribs</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="str">
@@ -984,11 +752,10 @@
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="str">
         <f aca="false">+'[1]Precios y Menú'!I6</f>
-        <v>
-Matambre a la pizza</v>
+        <v>Matambre a la pizza</v>
       </c>
       <c r="B20" s="8"/>
     </row>
@@ -999,11 +766,10 @@
       </c>
       <c r="B21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="str">
         <f aca="false">+'[1]Precios y Menú'!I8</f>
-        <v>
-Roast beef a la cerveza negra</v>
+        <v>Roast beef a la cerveza negra</v>
       </c>
       <c r="B22" s="8"/>
     </row>
@@ -1040,7 +806,7 @@
         <f aca="false">+'[1]Precios y Menú'!I13</f>
         <v>Gnocchis de papa con goulash</v>
       </c>
-      <c r="B27" s="10"/>
+      <c r="B27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="str">
@@ -1110,7 +876,7 @@
         <f aca="false">+'[1]Precios y Menú'!I23</f>
         <v>Puré de papas</v>
       </c>
-      <c r="B37" s="12"/>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="str">
@@ -1215,7 +981,7 @@
         <f aca="false">+'[1]Precios y Menú'!I38</f>
         <v>Promo 1 Entrada</v>
       </c>
-      <c r="B52" s="14"/>
+      <c r="B52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="13" t="str">
@@ -1279,6 +1045,9 @@
         <v>Promo 2 Bebidas</v>
       </c>
       <c r="B61" s="14"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1292,17 +1061,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="3.22"/>
@@ -1313,7 +1082,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="3.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="15" width="9.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="15" width="14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="27" style="15" width="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1457,7 +1226,7 @@
       </c>
       <c r="G6" s="22" t="n">
         <f aca="true">+TODAY()</f>
-        <v>44207</v>
+        <v>44223</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>

</xml_diff>

<commit_message>
ya se agregan todos los atributos intrinsecos del pedido, faltan los productos
</commit_message>
<xml_diff>
--- a/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
+++ b/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
@@ -150,6 +150,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -171,24 +172,28 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -196,6 +201,7 @@
       <color rgb="FF000000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -203,12 +209,14 @@
       <color rgb="FF000000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Monserrat light"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -626,10 +634,10 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.11"/>
@@ -1226,7 +1234,7 @@
       </c>
       <c r="G6" s="22" t="n">
         <f aca="true">+TODAY()</f>
-        <v>44223</v>
+        <v>44227</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>

</xml_diff>

<commit_message>
Arreglado para que se agrupe por productos para que se escriba bien la cantidad y tambien arreglado para que escriba en la columna correcta usando el id de pedido
</commit_message>
<xml_diff>
--- a/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
+++ b/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
@@ -144,7 +144,7 @@
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="\ * #,##0.00\ ;\ * \-#,##0.00\ ;\ * \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,13 +166,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -365,12 +358,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,23 +372,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,7 +392,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,7 +400,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,7 +408,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,123 +416,123 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,10 +620,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -659,403 +648,400 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="str">
+      <c r="A17" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I3</f>
         <v>BBQ Ribs</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="str">
+      <c r="A18" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I4</f>
         <v>Bife de Chorizo al Marsala</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="str">
+      <c r="A19" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I5</f>
         <v>Bondiola teriyaki</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="str">
+      <c r="A20" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I6</f>
         <v>Matambre a la pizza</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="str">
+      <c r="A21" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I7</f>
         <v>Matambrito de cerdo al verdeo</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="str">
+      <c r="A22" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I8</f>
         <v>Roast beef a la cerveza negra</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="str">
+      <c r="A23" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I9</f>
         <v>Solomillo de cerdo laqueado</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="str">
+      <c r="A24" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I10</f>
         <v>Premium 8</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="str">
+      <c r="A25" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I11</f>
         <v>Premium 9</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="str">
+      <c r="A26" s="6" t="str">
         <f aca="false">+'[1]Precios y Menú'!I12</f>
         <v>Premium 10</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="str">
+      <c r="A27" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I13</f>
         <v>Gnocchis de papa con goulash</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="str">
+      <c r="A28" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I14</f>
         <v>Milanesitas de cerdo a la napolitana</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="str">
+      <c r="A29" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I15</f>
         <v>Pata muslo al verdeo</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="str">
+      <c r="A30" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I16</f>
         <v>Pollo al ajillo</v>
       </c>
-      <c r="B30" s="10"/>
+      <c r="B30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="str">
+      <c r="A31" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I17</f>
         <v>Spaghetti con puttanesca</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="str">
+      <c r="A32" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I18</f>
         <v>Strogonoff de ternera</v>
       </c>
-      <c r="B32" s="10"/>
+      <c r="B32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="str">
+      <c r="A33" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I19</f>
         <v>Suprema con mostaza y miel</v>
       </c>
-      <c r="B33" s="10"/>
+      <c r="B33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="str">
+      <c r="A34" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I20</f>
         <v>Daily 18</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="str">
+      <c r="A35" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I21</f>
         <v>Daily 19</v>
       </c>
-      <c r="B35" s="10"/>
+      <c r="B35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="str">
+      <c r="A36" s="8" t="str">
         <f aca="false">+'[1]Precios y Menú'!I22</f>
         <v>Daily 20</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="str">
+      <c r="A37" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I23</f>
         <v>Puré de papas</v>
       </c>
-      <c r="B37" s="10"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="str">
+      <c r="A38" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I24</f>
         <v>Puré de batatas</v>
       </c>
-      <c r="B38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="str">
+      <c r="A39" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I25</f>
         <v>Arroz salteado con huevo, sésamo y cebollita de verdeo</v>
       </c>
-      <c r="B39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="str">
+      <c r="A40" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I26</f>
         <v>Milhojas de papa</v>
       </c>
-      <c r="B40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="str">
+      <c r="A41" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I27</f>
         <v>Batatas cuña</v>
       </c>
-      <c r="B41" s="12"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="11" t="str">
+      <c r="A42" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I28</f>
         <v>Cebollas Caramelizadas</v>
       </c>
-      <c r="B42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="11" t="str">
+      <c r="A43" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I29</f>
         <v>Focaccia al romero</v>
       </c>
-      <c r="B43" s="12"/>
+      <c r="B43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="11" t="str">
+      <c r="A44" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I30</f>
         <v>Kabutea con puerros</v>
       </c>
-      <c r="B44" s="12"/>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="11" t="str">
+      <c r="A45" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I31</f>
         <v>Guarnición 29</v>
       </c>
-      <c r="B45" s="12"/>
+      <c r="B45" s="11"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="11" t="str">
+      <c r="A46" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I32</f>
         <v>Guarnición 30</v>
       </c>
-      <c r="B46" s="12"/>
+      <c r="B46" s="11"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="11" t="str">
+      <c r="A47" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I33</f>
         <v>Guarnición 31</v>
       </c>
-      <c r="B47" s="12"/>
+      <c r="B47" s="11"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="11" t="str">
+      <c r="A48" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I34</f>
         <v>Guarnición 32</v>
       </c>
-      <c r="B48" s="12"/>
+      <c r="B48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11" t="str">
+      <c r="A49" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I35</f>
         <v>Guarnición 33</v>
       </c>
-      <c r="B49" s="12"/>
+      <c r="B49" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11" t="str">
+      <c r="A50" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I36</f>
         <v>Guarnición 34</v>
       </c>
-      <c r="B50" s="12"/>
+      <c r="B50" s="11"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11" t="str">
+      <c r="A51" s="10" t="str">
         <f aca="false">+'[1]Precios y Menú'!I37</f>
         <v>Guarnición 35</v>
       </c>
-      <c r="B51" s="12"/>
+      <c r="B51" s="11"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="13" t="str">
+      <c r="A52" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I38</f>
         <v>Promo 1 Entrada</v>
       </c>
-      <c r="B52" s="12"/>
+      <c r="B52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="13" t="str">
+      <c r="A53" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I39</f>
         <v>Promo 1 Principal</v>
       </c>
-      <c r="B53" s="14"/>
+      <c r="B53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="13" t="str">
+      <c r="A54" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I40</f>
         <v>Promo 1 Guarnición</v>
       </c>
-      <c r="B54" s="14"/>
+      <c r="B54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="13" t="str">
+      <c r="A55" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I41</f>
         <v>Promo 1 Salsas</v>
       </c>
-      <c r="B55" s="14"/>
+      <c r="B55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="13" t="str">
+      <c r="A56" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I42</f>
         <v>Promo 1 Bebidas</v>
       </c>
-      <c r="B56" s="14"/>
+      <c r="B56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="13" t="str">
+      <c r="A57" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I43</f>
         <v>Promo 2 Entrada</v>
       </c>
-      <c r="B57" s="14"/>
+      <c r="B57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="str">
+      <c r="A58" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I44</f>
         <v>Promo 2 Principal</v>
       </c>
-      <c r="B58" s="14"/>
+      <c r="B58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="13" t="str">
+      <c r="A59" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I45</f>
         <v>Promo 2 Guarnición</v>
       </c>
-      <c r="B59" s="14"/>
+      <c r="B59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="str">
+      <c r="A60" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I46</f>
         <v>Promo 2 Salsas</v>
       </c>
-      <c r="B60" s="14"/>
+      <c r="B60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="13" t="str">
+      <c r="A61" s="12" t="str">
         <f aca="false">+'[1]Precios y Menú'!I47</f>
         <v>Promo 2 Bebidas</v>
       </c>
-      <c r="B61" s="14"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="14"/>
+      <c r="B61" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1081,741 +1067,741 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="3.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="27.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="15" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="3.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="15" width="9.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="27" style="15" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="3.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="27.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="14" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="14" width="3.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="14" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="14" width="9.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="27" style="14" width="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16"/>
-      <c r="C3" s="17" t="s">
+      <c r="A3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16"/>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="15"/>
+      <c r="C4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20" t="s">
+      <c r="A6" s="15"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="22" t="n">
+      <c r="G6" s="21" t="n">
         <f aca="true">+TODAY()</f>
         <v>44227</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="C7" s="23" t="s">
+      <c r="A7" s="15"/>
+      <c r="C7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="20" t="n">
+      <c r="D7" s="19" t="e">
+        <f aca="false">+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="21"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="C8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="19" t="n">
         <f aca="false">+Pedido!B1</f>
         <v>0</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="22"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="C8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="20" t="n">
-        <f aca="false">+Pedido!B2</f>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="21"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15"/>
+      <c r="C11" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="25" t="n">
+        <f aca="false">+Pedido!B9</f>
         <v>0</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="22"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
-      <c r="C11" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="26" t="n">
+      <c r="F11" s="25" t="n">
+        <v>1699</v>
+      </c>
+      <c r="G11" s="25" t="n">
+        <f aca="false">+E11*F11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15"/>
+      <c r="C12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="28" t="n">
         <f aca="false">+Pedido!B10</f>
         <v>0</v>
       </c>
-      <c r="F11" s="26" t="n">
-        <v>1699</v>
-      </c>
-      <c r="G11" s="26" t="n">
-        <f aca="false">+E11*F11</f>
+      <c r="F12" s="28" t="n">
+        <v>1449</v>
+      </c>
+      <c r="G12" s="28" t="n">
+        <f aca="false">+E12*F12</f>
         <v>0</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I12" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="C12" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="29" t="n">
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15"/>
+      <c r="C13" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="28" t="n">
         <f aca="false">+Pedido!B11</f>
         <v>0</v>
       </c>
-      <c r="F12" s="29" t="n">
-        <v>1449</v>
-      </c>
-      <c r="G12" s="29" t="n">
-        <f aca="false">+E12*F12</f>
+      <c r="F13" s="28" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G13" s="28" t="n">
+        <f aca="false">+E13*F13</f>
         <v>0</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I13" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
-      <c r="C13" s="28" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="29" t="n">
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15"/>
+      <c r="C14" s="27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="28" t="n">
         <f aca="false">+Pedido!B12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="29" t="n">
-        <v>1299</v>
-      </c>
-      <c r="G13" s="29" t="n">
-        <f aca="false">+E13*F13</f>
+      <c r="F14" s="28" t="n">
+        <v>390</v>
+      </c>
+      <c r="G14" s="28" t="n">
+        <f aca="false">+E14*F14</f>
         <v>0</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16"/>
-      <c r="C14" s="28" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="29" t="n">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15"/>
+      <c r="C15" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="28" t="n">
         <f aca="false">+Pedido!B13</f>
         <v>0</v>
       </c>
-      <c r="F14" s="29" t="n">
-        <v>390</v>
-      </c>
-      <c r="G14" s="29" t="n">
-        <f aca="false">+E14*F14</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16"/>
-      <c r="C15" s="28" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="29" t="n">
-        <f aca="false">+Pedido!B14</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="29" t="n">
+      <c r="F15" s="28" t="n">
         <v>325</v>
       </c>
-      <c r="G15" s="29" t="n">
+      <c r="G15" s="28" t="n">
         <f aca="false">+E15*F15</f>
         <v>0</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="16"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16"/>
-      <c r="C16" s="30" t="n">
+      <c r="A16" s="15"/>
+      <c r="C16" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31" t="n">
+      <c r="E16" s="30"/>
+      <c r="F16" s="30" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="31" t="n">
+      <c r="G16" s="30" t="n">
         <f aca="false">+E16*F16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="16"/>
+      <c r="A17" s="15"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16"/>
-      <c r="C18" s="32"/>
-      <c r="F18" s="33" t="s">
+      <c r="A18" s="15"/>
+      <c r="C18" s="31"/>
+      <c r="F18" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="34" t="n">
+      <c r="G18" s="33" t="n">
         <v>250</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="16"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="16"/>
-      <c r="Y19" s="16"/>
-      <c r="Z19" s="16"/>
+      <c r="A19" s="15"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16"/>
-      <c r="C20" s="32"/>
-      <c r="F20" s="33" t="s">
+      <c r="A20" s="15"/>
+      <c r="C20" s="31"/>
+      <c r="F20" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="34" t="n">
+      <c r="G20" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="16"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
+      <c r="A21" s="15"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="40" t="n">
+      <c r="G22" s="39" t="n">
         <f aca="false">+SUM(G11:G20)</f>
         <v>250</v>
       </c>
-      <c r="H22" s="36"/>
-      <c r="I22" s="27" t="s">
+      <c r="H22" s="35"/>
+      <c r="I22" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="35"/>
-      <c r="Z22" s="35"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="34"/>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="16"/>
+      <c r="A23" s="15"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
ya agarra bien los combos, falta ver que agarre bien la formula
</commit_message>
<xml_diff>
--- a/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
+++ b/Pedidos/2021/012020/Generador de pedidos/Pedidos/Planilla Cliente.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t xml:space="preserve">Pedido</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">Promo del mes 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puré de batata</t>
   </si>
   <si>
     <t xml:space="preserve">SMART FOOD SOLUTIONS</t>
@@ -622,8 +625,8 @@
   </sheetPr>
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -876,9 +879,8 @@
       <c r="B37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="str">
-        <f aca="false">+'[1]Precios y Menú'!I24</f>
-        <v>Puré de batatas</v>
+      <c r="A38" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="B38" s="11"/>
     </row>
@@ -1061,7 +1063,7 @@
   </sheetPr>
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -1131,7 +1133,7 @@
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15"/>
       <c r="C3" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -1159,7 +1161,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15"/>
       <c r="C4" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1216,11 +1218,11 @@
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="21" t="n">
         <f aca="true">+TODAY()</f>
-        <v>44227</v>
+        <v>44230</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -1244,7 +1246,7 @@
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15"/>
       <c r="C7" s="22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="19" t="e">
         <f aca="false">+#REF!</f>
@@ -1275,7 +1277,7 @@
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15"/>
       <c r="C8" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="19" t="n">
         <f aca="false">+Pedido!B1</f>
@@ -1333,19 +1335,19 @@
       <c r="A10" s="23"/>
       <c r="B10" s="19"/>
       <c r="C10" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="23"/>
@@ -1387,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
@@ -1427,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
@@ -1467,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -1493,7 +1495,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" s="28" t="n">
         <f aca="false">+Pedido!B12</f>
@@ -1507,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -1533,7 +1535,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E15" s="28" t="n">
         <f aca="false">+Pedido!B13</f>
@@ -1547,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -1573,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30" t="n">
@@ -1584,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -1634,13 +1636,13 @@
       <c r="A18" s="15"/>
       <c r="C18" s="31"/>
       <c r="F18" s="32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G18" s="33" t="n">
         <v>250</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -1690,13 +1692,13 @@
       <c r="A20" s="15"/>
       <c r="C20" s="31"/>
       <c r="F20" s="32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G20" s="33" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -1749,7 +1751,7 @@
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
       <c r="F22" s="38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G22" s="39" t="n">
         <f aca="false">+SUM(G11:G20)</f>
@@ -1757,7 +1759,7 @@
       </c>
       <c r="H22" s="35"/>
       <c r="I22" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>

</xml_diff>